<commit_message>
[DEPLOY INSTAR STAGING]: v.0.1.48
</commit_message>
<xml_diff>
--- a/namc_customer_report.xlsx
+++ b/namc_customer_report.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\namc\namc-bug-db\react\app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE02EBE7-93E5-4073-A554-3B1001007BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47012056-DEC9-4651-A86A-CFDF92F74C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27165" yWindow="8775" windowWidth="21570" windowHeight="13035" xr2:uid="{85F6B590-B172-4F7F-B99D-007C43BEB306}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="19530" xr2:uid="{85F6B590-B172-4F7F-B99D-007C43BEB306}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Address1">Summary!$E$13</definedName>
-    <definedName name="Address2">Summary!$E$14</definedName>
-    <definedName name="CityStateZip">Summary!$E$15</definedName>
-    <definedName name="CustomerName">Summary!$E$12</definedName>
-    <definedName name="Email">Summary!$E$17</definedName>
-    <definedName name="ReportDate">Summary!$D$9</definedName>
-    <definedName name="SubmitterName">Summary!$E$11</definedName>
-    <definedName name="Telephone">Summary!$E$16</definedName>
+    <definedName name="Address1">Summary!$E$16</definedName>
+    <definedName name="Address2">Summary!$E$17</definedName>
+    <definedName name="CityStateZip">Summary!$E$18</definedName>
+    <definedName name="CustomerName">Summary!$E$15</definedName>
+    <definedName name="Email">Summary!$E$20</definedName>
+    <definedName name="ReportDate">Summary!$D$12</definedName>
+    <definedName name="SubmitterName">Summary!$E$14</definedName>
+    <definedName name="Telephone">Summary!$E$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>BLM/USU National Aquatic Monitoring Center (NAMC)</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Address:</t>
   </si>
   <si>
-    <t>Telelphone:</t>
-  </si>
-  <si>
     <t>Email:</t>
   </si>
   <si>
@@ -85,6 +82,21 @@
   </si>
   <si>
     <t>Click here for more information about the contents of this report and how it was generated.</t>
+  </si>
+  <si>
+    <t>Director:</t>
+  </si>
+  <si>
+    <t>Trip Armstrong</t>
+  </si>
+  <si>
+    <t>Telephone:</t>
+  </si>
+  <si>
+    <t>trip.armstrong@usu.edu</t>
+  </si>
+  <si>
+    <t>(760) 709-1210</t>
   </si>
 </sst>
 </file>
@@ -554,99 +566,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BDBCB3-947A-4E82-AAEF-BDC760B967B2}">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="2" t="s">
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{E7660F74-7B0C-43DE-9A6D-7D04D5FB59E1}"/>
+    <hyperlink ref="A24" r:id="rId1" xr:uid="{E7660F74-7B0C-43DE-9A6D-7D04D5FB59E1}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{77D11643-D07C-437C-B657-4BA021913FD1}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{CABCF87B-447B-44FF-B177-0D386A2379AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>